<commit_message>
Update employee DOB data again
</commit_message>
<xml_diff>
--- a/data/DOB.xlsx
+++ b/data/DOB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29819"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55C302BE-2F65-4A59-B1F0-3D292930A33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A78D6D62-C409-42A3-A2AD-090886FDF6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="3">
-        <v>37676</v>
+        <v>37678</v>
       </c>
       <c r="D2" s="1">
         <v>9999444422</v>
@@ -837,7 +837,7 @@
         <v>56</v>
       </c>
       <c r="C8" s="3">
-        <v>36216</v>
+        <v>36217</v>
       </c>
       <c r="D8" s="1">
         <v>9999444422</v>

</xml_diff>